<commit_message>
updated after review with Karen
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C34752
</commit_message>
<xml_diff>
--- a/Project Management/eCL OY4/CCO OY4_eCoaching Log TailorPlan Worksheet.xlsx
+++ b/Project Management/eCL OY4/CCO OY4_eCoaching Log TailorPlan Worksheet.xlsx
@@ -4714,6 +4714,15 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="82" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="82" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="82" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="82" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4726,22 +4735,73 @@
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="28" fillId="36" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4750,57 +4810,6 @@
     <xf numFmtId="49" fontId="28" fillId="36" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="60" xfId="43" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4851,15 +4860,6 @@
     </xf>
     <xf numFmtId="0" fontId="35" fillId="41" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="82" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="82" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="82" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="451">
@@ -6224,20 +6224,20 @@
       <c r="B2" s="8"/>
     </row>
     <row r="3" spans="1:2" s="6" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="323" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="323"/>
+      <c r="A3" s="326" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="326"/>
     </row>
     <row r="4" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9"/>
       <c r="B4" s="10"/>
     </row>
     <row r="5" spans="1:2" s="6" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="324" t="s">
+      <c r="A5" s="327" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="324"/>
+      <c r="B5" s="327"/>
     </row>
     <row r="6" spans="1:2" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10"/>
@@ -6396,10 +6396,10 @@
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="325" t="s">
+      <c r="A36" s="328" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="325"/>
+      <c r="B36" s="328"/>
     </row>
     <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="16"/>
@@ -6416,29 +6416,29 @@
       <c r="B39" s="17"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="326"/>
+      <c r="A40" s="329"/>
       <c r="B40" s="18" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="326"/>
+      <c r="A41" s="329"/>
       <c r="B41" s="19"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="326"/>
+      <c r="A42" s="329"/>
       <c r="B42" s="18" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="326"/>
+      <c r="A43" s="329"/>
       <c r="B43" s="18" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="326"/>
+      <c r="A44" s="329"/>
       <c r="B44" s="18" t="s">
         <v>28</v>
       </c>
@@ -6534,20 +6534,20 @@
       <c r="B3" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="342" t="s">
+      <c r="C3" s="330" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="343"/>
+      <c r="D3" s="331"/>
     </row>
     <row r="4" spans="1:11" s="6" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="344" t="s">
+      <c r="A4" s="332" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="345"/>
-      <c r="C4" s="346" t="s">
+      <c r="B4" s="333"/>
+      <c r="C4" s="334" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="347"/>
+      <c r="D4" s="335"/>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
     </row>
@@ -6556,10 +6556,10 @@
       <c r="B5" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="348" t="s">
+      <c r="C5" s="336" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="349"/>
+      <c r="D5" s="337"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -6569,14 +6569,14 @@
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" s="6" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="350" t="s">
+      <c r="A6" s="338" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="351"/>
-      <c r="C6" s="329" t="s">
+      <c r="B6" s="339"/>
+      <c r="C6" s="340" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="330"/>
+      <c r="D6" s="341"/>
       <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -6584,176 +6584,176 @@
         <v>42</v>
       </c>
       <c r="B7" s="31"/>
-      <c r="C7" s="329" t="s">
+      <c r="C7" s="340" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="330"/>
+      <c r="D7" s="341"/>
       <c r="E7" s="25"/>
     </row>
     <row r="8" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="335"/>
+      <c r="A8" s="342"/>
       <c r="B8" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="338" t="s">
+      <c r="C8" s="345" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="339"/>
+      <c r="D8" s="346"/>
       <c r="E8" s="33"/>
     </row>
     <row r="9" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="336"/>
+      <c r="A9" s="343"/>
       <c r="B9" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="331" t="s">
+      <c r="C9" s="347" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="332"/>
+      <c r="D9" s="348"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="336"/>
+      <c r="A10" s="343"/>
       <c r="B10" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="331" t="s">
+      <c r="C10" s="347" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="332"/>
+      <c r="D10" s="348"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="336"/>
+      <c r="A11" s="343"/>
       <c r="B11" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="331" t="s">
+      <c r="C11" s="347" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="332"/>
+      <c r="D11" s="348"/>
     </row>
     <row r="12" spans="1:11" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="336"/>
+      <c r="A12" s="343"/>
       <c r="B12" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="327" t="s">
+      <c r="C12" s="349" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="328"/>
+      <c r="D12" s="350"/>
     </row>
     <row r="13" spans="1:11" s="6" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="336"/>
+      <c r="A13" s="343"/>
       <c r="B13" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="331" t="s">
+      <c r="C13" s="347" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="332"/>
+      <c r="D13" s="348"/>
       <c r="E13" s="1"/>
       <c r="F13" s="25"/>
     </row>
     <row r="14" spans="1:11" s="6" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="336"/>
+      <c r="A14" s="343"/>
       <c r="B14" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="340"/>
-      <c r="D14" s="341"/>
+      <c r="C14" s="351"/>
+      <c r="D14" s="352"/>
       <c r="E14" s="1"/>
       <c r="F14" s="25"/>
     </row>
     <row r="15" spans="1:11" s="6" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="336"/>
+      <c r="A15" s="343"/>
       <c r="B15" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="331" t="s">
+      <c r="C15" s="347" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="332"/>
+      <c r="D15" s="348"/>
       <c r="E15" s="1"/>
       <c r="F15" s="25"/>
     </row>
     <row r="16" spans="1:11" s="6" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="336"/>
+      <c r="A16" s="343"/>
       <c r="B16" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="331" t="s">
+      <c r="C16" s="347" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="332"/>
+      <c r="D16" s="348"/>
       <c r="E16" s="1"/>
       <c r="F16" s="25"/>
     </row>
     <row r="17" spans="1:6" s="6" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="336"/>
+      <c r="A17" s="343"/>
       <c r="B17" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="331" t="s">
+      <c r="C17" s="347" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="332"/>
+      <c r="D17" s="348"/>
       <c r="E17" s="1"/>
       <c r="F17" s="25"/>
     </row>
     <row r="18" spans="1:6" s="6" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="336"/>
+      <c r="A18" s="343"/>
       <c r="B18" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="331" t="s">
+      <c r="C18" s="347" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="332"/>
+      <c r="D18" s="348"/>
       <c r="E18" s="1"/>
       <c r="F18" s="25"/>
     </row>
     <row r="19" spans="1:6" s="37" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="336"/>
+      <c r="A19" s="343"/>
       <c r="B19" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="338" t="s">
+      <c r="C19" s="345" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="339"/>
+      <c r="D19" s="346"/>
       <c r="F19" s="33"/>
     </row>
     <row r="20" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="336"/>
+      <c r="A20" s="343"/>
       <c r="B20" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="331" t="s">
+      <c r="C20" s="347" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="332"/>
+      <c r="D20" s="348"/>
     </row>
     <row r="21" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="336"/>
+      <c r="A21" s="343"/>
       <c r="B21" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="327" t="s">
+      <c r="C21" s="349" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="328"/>
+      <c r="D21" s="350"/>
     </row>
     <row r="22" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="336"/>
+      <c r="A22" s="343"/>
       <c r="B22" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="331" t="s">
+      <c r="C22" s="347" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="332"/>
+      <c r="D22" s="348"/>
     </row>
     <row r="23" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="336"/>
+      <c r="A23" s="343"/>
       <c r="B23" s="34" t="s">
         <v>73</v>
       </c>
@@ -6763,119 +6763,119 @@
       <c r="D23" s="39"/>
     </row>
     <row r="24" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="336"/>
+      <c r="A24" s="343"/>
       <c r="B24" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="333" t="s">
+      <c r="C24" s="353" t="s">
         <v>76</v>
       </c>
-      <c r="D24" s="334"/>
+      <c r="D24" s="354"/>
     </row>
     <row r="25" spans="1:6" s="37" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="336"/>
+      <c r="A25" s="343"/>
       <c r="B25" s="34"/>
-      <c r="C25" s="331" t="s">
+      <c r="C25" s="347" t="s">
         <v>77</v>
       </c>
-      <c r="D25" s="332"/>
+      <c r="D25" s="348"/>
       <c r="E25" s="40"/>
     </row>
     <row r="26" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="336"/>
+      <c r="A26" s="343"/>
       <c r="B26" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="333" t="s">
+      <c r="C26" s="353" t="s">
         <v>79</v>
       </c>
-      <c r="D26" s="334"/>
+      <c r="D26" s="354"/>
     </row>
     <row r="27" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="336"/>
+      <c r="A27" s="343"/>
       <c r="B27" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="C27" s="327" t="s">
+      <c r="C27" s="349" t="s">
         <v>81</v>
       </c>
-      <c r="D27" s="328"/>
+      <c r="D27" s="350"/>
     </row>
     <row r="28" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="336"/>
+      <c r="A28" s="343"/>
       <c r="B28" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="C28" s="331" t="s">
+      <c r="C28" s="347" t="s">
         <v>83</v>
       </c>
-      <c r="D28" s="332"/>
+      <c r="D28" s="348"/>
     </row>
     <row r="29" spans="1:6" s="37" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="337"/>
+      <c r="A29" s="344"/>
       <c r="B29" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="C29" s="331" t="s">
+      <c r="C29" s="347" t="s">
         <v>85</v>
       </c>
-      <c r="D29" s="332"/>
+      <c r="D29" s="348"/>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="C30" s="331" t="s">
+      <c r="C30" s="347" t="s">
         <v>87</v>
       </c>
-      <c r="D30" s="332"/>
+      <c r="D30" s="348"/>
     </row>
     <row r="31" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="C31" s="331" t="s">
+      <c r="C31" s="347" t="s">
         <v>89</v>
       </c>
-      <c r="D31" s="332"/>
+      <c r="D31" s="348"/>
     </row>
     <row r="32" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="C32" s="331" t="s">
+      <c r="C32" s="347" t="s">
         <v>91</v>
       </c>
-      <c r="D32" s="332"/>
+      <c r="D32" s="348"/>
     </row>
     <row r="33" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="C33" s="331" t="s">
+      <c r="C33" s="347" t="s">
         <v>93</v>
       </c>
-      <c r="D33" s="332"/>
+      <c r="D33" s="348"/>
     </row>
     <row r="34" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="C34" s="331" t="s">
+      <c r="C34" s="347" t="s">
         <v>95</v>
       </c>
-      <c r="D34" s="332"/>
+      <c r="D34" s="348"/>
     </row>
     <row r="35" spans="1:6" s="6" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="C35" s="329" t="s">
+      <c r="C35" s="340" t="s">
         <v>97</v>
       </c>
-      <c r="D35" s="330"/>
+      <c r="D35" s="341"/>
       <c r="E35" s="1"/>
       <c r="F35" s="25"/>
     </row>
@@ -7061,12 +7061,19 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="A8:A29"/>
     <mergeCell ref="C8:D8"/>
@@ -7083,19 +7090,12 @@
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7116,9 +7116,9 @@
   <dimension ref="A1:AF184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B33" sqref="B33"/>
-      <selection pane="bottomLeft" activeCell="E148" sqref="E148"/>
+      <selection pane="bottomLeft" activeCell="D174" sqref="D174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7140,10 +7140,10 @@
       <c r="B1" s="213" t="s">
         <v>396</v>
       </c>
-      <c r="C1" s="352" t="s">
+      <c r="C1" s="355" t="s">
         <v>399</v>
       </c>
-      <c r="D1" s="352"/>
+      <c r="D1" s="355"/>
       <c r="E1" s="210" t="s">
         <v>397</v>
       </c>
@@ -9997,7 +9997,7 @@
       <c r="A71" s="65" t="s">
         <v>401</v>
       </c>
-      <c r="B71" s="353" t="s">
+      <c r="B71" s="356" t="s">
         <v>86</v>
       </c>
       <c r="C71" s="234" t="s">
@@ -10012,7 +10012,7 @@
       <c r="G71" s="235" t="s">
         <v>86</v>
       </c>
-      <c r="H71" s="354" t="s">
+      <c r="H71" s="357" t="s">
         <v>458</v>
       </c>
       <c r="AA71" s="319">
@@ -10040,7 +10040,7 @@
       <c r="A72" s="65" t="s">
         <v>457</v>
       </c>
-      <c r="B72" s="353"/>
+      <c r="B72" s="356"/>
       <c r="C72" s="234" t="s">
         <v>46</v>
       </c>
@@ -10053,7 +10053,7 @@
       <c r="G72" s="235" t="s">
         <v>86</v>
       </c>
-      <c r="H72" s="354"/>
+      <c r="H72" s="357"/>
       <c r="AA72" s="319">
         <f t="shared" si="5"/>
         <v>1</v>
@@ -10079,7 +10079,7 @@
       <c r="A73" s="65" t="s">
         <v>459</v>
       </c>
-      <c r="B73" s="353"/>
+      <c r="B73" s="356"/>
       <c r="C73" s="234" t="s">
         <v>50</v>
       </c>
@@ -10092,7 +10092,7 @@
       <c r="G73" s="235" t="s">
         <v>86</v>
       </c>
-      <c r="H73" s="354"/>
+      <c r="H73" s="357"/>
       <c r="AA73" s="319">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -10199,7 +10199,7 @@
       <c r="A76" s="65" t="s">
         <v>401</v>
       </c>
-      <c r="B76" s="353" t="s">
+      <c r="B76" s="356" t="s">
         <v>86</v>
       </c>
       <c r="C76" s="234" t="s">
@@ -10214,7 +10214,7 @@
       <c r="G76" s="235" t="s">
         <v>86</v>
       </c>
-      <c r="H76" s="355" t="s">
+      <c r="H76" s="358" t="s">
         <v>458</v>
       </c>
       <c r="AA76" s="319">
@@ -10242,7 +10242,7 @@
       <c r="A77" s="65" t="s">
         <v>457</v>
       </c>
-      <c r="B77" s="353"/>
+      <c r="B77" s="356"/>
       <c r="C77" s="234" t="s">
         <v>46</v>
       </c>
@@ -10255,7 +10255,7 @@
       <c r="G77" s="235" t="s">
         <v>86</v>
       </c>
-      <c r="H77" s="355"/>
+      <c r="H77" s="358"/>
       <c r="AA77" s="319">
         <f t="shared" si="5"/>
         <v>1</v>
@@ -10281,7 +10281,7 @@
       <c r="A78" s="65" t="s">
         <v>459</v>
       </c>
-      <c r="B78" s="353"/>
+      <c r="B78" s="356"/>
       <c r="C78" s="234" t="s">
         <v>50</v>
       </c>
@@ -10294,7 +10294,7 @@
       <c r="G78" s="235" t="s">
         <v>86</v>
       </c>
-      <c r="H78" s="355"/>
+      <c r="H78" s="358"/>
       <c r="AA78" s="319">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -13141,9 +13141,9 @@
         <v>1</v>
       </c>
       <c r="E148" s="318" t="s">
-        <v>67</v>
-      </c>
-      <c r="F148" s="369" t="s">
+        <v>71</v>
+      </c>
+      <c r="F148" s="323" t="s">
         <v>520</v>
       </c>
       <c r="G148" s="235" t="s">
@@ -13154,7 +13154,7 @@
       </c>
       <c r="AA148" s="319">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB148" s="319">
         <f t="shared" si="11"/>
@@ -13162,7 +13162,7 @@
       </c>
       <c r="AC148" s="319">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD148" s="319">
         <f t="shared" si="13"/>
@@ -13184,9 +13184,9 @@
         <v>1</v>
       </c>
       <c r="E149" s="318" t="s">
-        <v>67</v>
-      </c>
-      <c r="F149" s="370" t="s">
+        <v>71</v>
+      </c>
+      <c r="F149" s="324" t="s">
         <v>520</v>
       </c>
       <c r="G149" s="235" t="s">
@@ -13197,7 +13197,7 @@
       </c>
       <c r="AA149" s="319">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB149" s="319">
         <f t="shared" si="11"/>
@@ -13205,7 +13205,7 @@
       </c>
       <c r="AC149" s="319">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD149" s="319">
         <f t="shared" si="13"/>
@@ -13227,9 +13227,9 @@
         <v>1</v>
       </c>
       <c r="E150" s="318" t="s">
-        <v>67</v>
-      </c>
-      <c r="F150" s="371" t="s">
+        <v>71</v>
+      </c>
+      <c r="F150" s="325" t="s">
         <v>520</v>
       </c>
       <c r="G150" s="235" t="s">
@@ -13240,7 +13240,7 @@
       </c>
       <c r="AA150" s="319">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB150" s="319">
         <f t="shared" si="11"/>
@@ -13248,7 +13248,7 @@
       </c>
       <c r="AC150" s="319">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD150" s="319">
         <f t="shared" si="13"/>
@@ -13263,7 +13263,7 @@
       <c r="A151" s="65" t="s">
         <v>401</v>
       </c>
-      <c r="B151" s="353" t="s">
+      <c r="B151" s="356" t="s">
         <v>86</v>
       </c>
       <c r="C151" s="234" t="s">
@@ -13278,7 +13278,7 @@
       <c r="G151" s="235" t="s">
         <v>86</v>
       </c>
-      <c r="H151" s="354" t="s">
+      <c r="H151" s="357" t="s">
         <v>458</v>
       </c>
       <c r="AA151" s="319">
@@ -13306,7 +13306,7 @@
       <c r="A152" s="65" t="s">
         <v>457</v>
       </c>
-      <c r="B152" s="353"/>
+      <c r="B152" s="356"/>
       <c r="C152" s="234" t="s">
         <v>46</v>
       </c>
@@ -13319,7 +13319,7 @@
       <c r="G152" s="235" t="s">
         <v>86</v>
       </c>
-      <c r="H152" s="354"/>
+      <c r="H152" s="357"/>
       <c r="AA152" s="319">
         <f t="shared" si="10"/>
         <v>1</v>
@@ -13345,7 +13345,7 @@
       <c r="A153" s="65" t="s">
         <v>459</v>
       </c>
-      <c r="B153" s="353"/>
+      <c r="B153" s="356"/>
       <c r="C153" s="234" t="s">
         <v>50</v>
       </c>
@@ -13358,7 +13358,7 @@
       <c r="G153" s="235" t="s">
         <v>86</v>
       </c>
-      <c r="H153" s="354"/>
+      <c r="H153" s="357"/>
       <c r="AA153" s="319">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -14162,7 +14162,7 @@
         <v>1</v>
       </c>
       <c r="E173" s="53" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G173" s="73" t="s">
         <v>228</v>
@@ -14172,7 +14172,7 @@
       </c>
       <c r="AA173" s="319">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB173" s="319">
         <f t="shared" si="11"/>
@@ -14180,7 +14180,7 @@
       </c>
       <c r="AC173" s="319">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD173" s="319">
         <f t="shared" si="13"/>
@@ -14202,7 +14202,7 @@
       <c r="H174" s="238"/>
       <c r="AA174" s="82">
         <f>SUM(AA4:AA173)</f>
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AB174" s="82">
         <f>SUM(AB4:AB173)</f>
@@ -14210,7 +14210,7 @@
       </c>
       <c r="AC174" s="82">
         <f>SUM(AC4:AC173)</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AD174" s="82">
         <f>SUM(AD4:AD173)</f>
@@ -14237,11 +14237,11 @@
       <c r="D178" s="73"/>
       <c r="E178" s="84">
         <f>AA174/F184</f>
-        <v>0.75</v>
+        <v>0.73750000000000004</v>
       </c>
       <c r="F178">
         <f>AA174</f>
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
@@ -14267,11 +14267,11 @@
       <c r="D180" s="73"/>
       <c r="E180" s="84">
         <f>AC174/F184</f>
-        <v>9.375E-2</v>
+        <v>0.10625</v>
       </c>
       <c r="F180">
         <f>AC174</f>
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.2">
@@ -15279,19 +15279,19 @@
       <c r="QL2" s="89"/>
     </row>
     <row r="3" spans="1:454" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="356" t="s">
+      <c r="A3" s="359" t="s">
         <v>256</v>
       </c>
-      <c r="B3" s="357"/>
-      <c r="C3" s="357"/>
-      <c r="D3" s="357"/>
-      <c r="E3" s="357"/>
-      <c r="F3" s="357"/>
-      <c r="G3" s="357"/>
-      <c r="H3" s="357"/>
-      <c r="I3" s="357"/>
-      <c r="J3" s="357"/>
-      <c r="K3" s="357"/>
+      <c r="B3" s="360"/>
+      <c r="C3" s="360"/>
+      <c r="D3" s="360"/>
+      <c r="E3" s="360"/>
+      <c r="F3" s="360"/>
+      <c r="G3" s="360"/>
+      <c r="H3" s="360"/>
+      <c r="I3" s="360"/>
+      <c r="J3" s="360"/>
+      <c r="K3" s="360"/>
     </row>
     <row r="4" spans="1:454" s="85" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="93" t="s">
@@ -16873,18 +16873,18 @@
       <c r="QK2" s="89"/>
     </row>
     <row r="3" spans="1:453" s="85" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="356" t="s">
+      <c r="A3" s="359" t="s">
         <v>299</v>
       </c>
-      <c r="B3" s="357"/>
-      <c r="C3" s="357"/>
-      <c r="D3" s="357"/>
-      <c r="E3" s="357"/>
-      <c r="F3" s="357"/>
-      <c r="G3" s="357"/>
-      <c r="H3" s="357"/>
-      <c r="I3" s="357"/>
-      <c r="J3" s="358"/>
+      <c r="B3" s="360"/>
+      <c r="C3" s="360"/>
+      <c r="D3" s="360"/>
+      <c r="E3" s="360"/>
+      <c r="F3" s="360"/>
+      <c r="G3" s="360"/>
+      <c r="H3" s="360"/>
+      <c r="I3" s="360"/>
+      <c r="J3" s="361"/>
     </row>
     <row r="4" spans="1:453" s="85" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="97"/>
@@ -18018,47 +18018,47 @@
     </row>
     <row r="3" spans="1:30" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="150"/>
-      <c r="C3" s="361" t="s">
+      <c r="C3" s="364" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="362"/>
-      <c r="E3" s="362"/>
-      <c r="F3" s="363"/>
-      <c r="G3" s="361" t="s">
+      <c r="D3" s="365"/>
+      <c r="E3" s="365"/>
+      <c r="F3" s="366"/>
+      <c r="G3" s="364" t="s">
         <v>110</v>
       </c>
-      <c r="H3" s="362"/>
-      <c r="I3" s="362"/>
-      <c r="J3" s="362"/>
-      <c r="K3" s="362"/>
-      <c r="L3" s="362"/>
-      <c r="M3" s="364" t="s">
+      <c r="H3" s="365"/>
+      <c r="I3" s="365"/>
+      <c r="J3" s="365"/>
+      <c r="K3" s="365"/>
+      <c r="L3" s="365"/>
+      <c r="M3" s="367" t="s">
         <v>80</v>
       </c>
-      <c r="N3" s="365"/>
-      <c r="O3" s="359" t="s">
+      <c r="N3" s="368"/>
+      <c r="O3" s="362" t="s">
         <v>84</v>
       </c>
-      <c r="P3" s="366"/>
-      <c r="Q3" s="366"/>
-      <c r="R3" s="366"/>
-      <c r="S3" s="366"/>
-      <c r="T3" s="360"/>
-      <c r="U3" s="367" t="s">
+      <c r="P3" s="369"/>
+      <c r="Q3" s="369"/>
+      <c r="R3" s="369"/>
+      <c r="S3" s="369"/>
+      <c r="T3" s="363"/>
+      <c r="U3" s="370" t="s">
         <v>367</v>
       </c>
-      <c r="V3" s="368"/>
-      <c r="W3" s="359" t="s">
+      <c r="V3" s="371"/>
+      <c r="W3" s="362" t="s">
         <v>94</v>
       </c>
-      <c r="X3" s="366"/>
-      <c r="Y3" s="366"/>
-      <c r="Z3" s="366"/>
-      <c r="AA3" s="360"/>
-      <c r="AB3" s="359" t="s">
+      <c r="X3" s="369"/>
+      <c r="Y3" s="369"/>
+      <c r="Z3" s="369"/>
+      <c r="AA3" s="363"/>
+      <c r="AB3" s="362" t="s">
         <v>228</v>
       </c>
-      <c r="AC3" s="360"/>
+      <c r="AC3" s="363"/>
       <c r="AD3" s="85"/>
     </row>
     <row r="4" spans="1:30" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -19226,6 +19226,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Unknown Document Type" ma:contentTypeID="0x010104" ma:contentTypeVersion="0" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="05d83ceaa0bbd2e3bc716e6e66bd857a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b3d69fe45253d5ff147bb69036b756a7">
     <xsd:element name="properties">
@@ -19339,15 +19348,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -19355,6 +19355,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60846BC6-3376-492B-A137-BE9B817BCED1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD7F02ED-4036-4861-BDC4-1969BAC60D5E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19366,14 +19374,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60846BC6-3376-492B-A137-BE9B817BCED1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
update after review with Karen
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C34763
</commit_message>
<xml_diff>
--- a/Project Management/eCL OY4/CCO OY4_eCoaching Log TailorPlan Worksheet.xlsx
+++ b/Project Management/eCL OY4/CCO OY4_eCoaching Log TailorPlan Worksheet.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1304" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="521">
   <si>
     <t>Purpose of this worksheet</t>
   </si>
@@ -4735,6 +4735,51 @@
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="36" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="36" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -4763,51 +4808,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="36" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="36" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="60" xfId="43" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6534,20 +6534,20 @@
       <c r="B3" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="330" t="s">
+      <c r="C3" s="345" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="331"/>
+      <c r="D3" s="346"/>
     </row>
     <row r="4" spans="1:11" s="6" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="332" t="s">
+      <c r="A4" s="347" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="333"/>
-      <c r="C4" s="334" t="s">
+      <c r="B4" s="348"/>
+      <c r="C4" s="349" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="335"/>
+      <c r="D4" s="350"/>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
     </row>
@@ -6556,10 +6556,10 @@
       <c r="B5" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="336" t="s">
+      <c r="C5" s="351" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="337"/>
+      <c r="D5" s="352"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -6569,14 +6569,14 @@
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" s="6" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="338" t="s">
+      <c r="A6" s="353" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="339"/>
-      <c r="C6" s="340" t="s">
+      <c r="B6" s="354"/>
+      <c r="C6" s="332" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="341"/>
+      <c r="D6" s="333"/>
       <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -6584,176 +6584,176 @@
         <v>42</v>
       </c>
       <c r="B7" s="31"/>
-      <c r="C7" s="340" t="s">
+      <c r="C7" s="332" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="341"/>
+      <c r="D7" s="333"/>
       <c r="E7" s="25"/>
     </row>
     <row r="8" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="342"/>
+      <c r="A8" s="338"/>
       <c r="B8" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="345" t="s">
+      <c r="C8" s="341" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="346"/>
+      <c r="D8" s="342"/>
       <c r="E8" s="33"/>
     </row>
     <row r="9" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="343"/>
+      <c r="A9" s="339"/>
       <c r="B9" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="347" t="s">
+      <c r="C9" s="334" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="348"/>
+      <c r="D9" s="335"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="343"/>
+      <c r="A10" s="339"/>
       <c r="B10" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="347" t="s">
+      <c r="C10" s="334" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="348"/>
+      <c r="D10" s="335"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="343"/>
+      <c r="A11" s="339"/>
       <c r="B11" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="347" t="s">
+      <c r="C11" s="334" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="348"/>
+      <c r="D11" s="335"/>
     </row>
     <row r="12" spans="1:11" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="343"/>
+      <c r="A12" s="339"/>
       <c r="B12" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="349" t="s">
+      <c r="C12" s="330" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="350"/>
+      <c r="D12" s="331"/>
     </row>
     <row r="13" spans="1:11" s="6" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="343"/>
+      <c r="A13" s="339"/>
       <c r="B13" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="347" t="s">
+      <c r="C13" s="334" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="348"/>
+      <c r="D13" s="335"/>
       <c r="E13" s="1"/>
       <c r="F13" s="25"/>
     </row>
     <row r="14" spans="1:11" s="6" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="343"/>
+      <c r="A14" s="339"/>
       <c r="B14" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="351"/>
-      <c r="D14" s="352"/>
+      <c r="C14" s="343"/>
+      <c r="D14" s="344"/>
       <c r="E14" s="1"/>
       <c r="F14" s="25"/>
     </row>
     <row r="15" spans="1:11" s="6" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="343"/>
+      <c r="A15" s="339"/>
       <c r="B15" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="347" t="s">
+      <c r="C15" s="334" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="348"/>
+      <c r="D15" s="335"/>
       <c r="E15" s="1"/>
       <c r="F15" s="25"/>
     </row>
     <row r="16" spans="1:11" s="6" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="343"/>
+      <c r="A16" s="339"/>
       <c r="B16" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="347" t="s">
+      <c r="C16" s="334" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="348"/>
+      <c r="D16" s="335"/>
       <c r="E16" s="1"/>
       <c r="F16" s="25"/>
     </row>
     <row r="17" spans="1:6" s="6" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="343"/>
+      <c r="A17" s="339"/>
       <c r="B17" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="347" t="s">
+      <c r="C17" s="334" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="348"/>
+      <c r="D17" s="335"/>
       <c r="E17" s="1"/>
       <c r="F17" s="25"/>
     </row>
     <row r="18" spans="1:6" s="6" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="343"/>
+      <c r="A18" s="339"/>
       <c r="B18" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="347" t="s">
+      <c r="C18" s="334" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="348"/>
+      <c r="D18" s="335"/>
       <c r="E18" s="1"/>
       <c r="F18" s="25"/>
     </row>
     <row r="19" spans="1:6" s="37" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="343"/>
+      <c r="A19" s="339"/>
       <c r="B19" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="345" t="s">
+      <c r="C19" s="341" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="346"/>
+      <c r="D19" s="342"/>
       <c r="F19" s="33"/>
     </row>
     <row r="20" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="343"/>
+      <c r="A20" s="339"/>
       <c r="B20" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="347" t="s">
+      <c r="C20" s="334" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="348"/>
+      <c r="D20" s="335"/>
     </row>
     <row r="21" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="343"/>
+      <c r="A21" s="339"/>
       <c r="B21" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="349" t="s">
+      <c r="C21" s="330" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="350"/>
+      <c r="D21" s="331"/>
     </row>
     <row r="22" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="343"/>
+      <c r="A22" s="339"/>
       <c r="B22" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="347" t="s">
+      <c r="C22" s="334" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="348"/>
+      <c r="D22" s="335"/>
     </row>
     <row r="23" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="343"/>
+      <c r="A23" s="339"/>
       <c r="B23" s="34" t="s">
         <v>73</v>
       </c>
@@ -6763,119 +6763,119 @@
       <c r="D23" s="39"/>
     </row>
     <row r="24" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="343"/>
+      <c r="A24" s="339"/>
       <c r="B24" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="353" t="s">
+      <c r="C24" s="336" t="s">
         <v>76</v>
       </c>
-      <c r="D24" s="354"/>
+      <c r="D24" s="337"/>
     </row>
     <row r="25" spans="1:6" s="37" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="343"/>
+      <c r="A25" s="339"/>
       <c r="B25" s="34"/>
-      <c r="C25" s="347" t="s">
+      <c r="C25" s="334" t="s">
         <v>77</v>
       </c>
-      <c r="D25" s="348"/>
+      <c r="D25" s="335"/>
       <c r="E25" s="40"/>
     </row>
     <row r="26" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="343"/>
+      <c r="A26" s="339"/>
       <c r="B26" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="353" t="s">
+      <c r="C26" s="336" t="s">
         <v>79</v>
       </c>
-      <c r="D26" s="354"/>
+      <c r="D26" s="337"/>
     </row>
     <row r="27" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="343"/>
+      <c r="A27" s="339"/>
       <c r="B27" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="C27" s="349" t="s">
+      <c r="C27" s="330" t="s">
         <v>81</v>
       </c>
-      <c r="D27" s="350"/>
+      <c r="D27" s="331"/>
     </row>
     <row r="28" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="343"/>
+      <c r="A28" s="339"/>
       <c r="B28" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="C28" s="347" t="s">
+      <c r="C28" s="334" t="s">
         <v>83</v>
       </c>
-      <c r="D28" s="348"/>
+      <c r="D28" s="335"/>
     </row>
     <row r="29" spans="1:6" s="37" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="344"/>
+      <c r="A29" s="340"/>
       <c r="B29" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="C29" s="347" t="s">
+      <c r="C29" s="334" t="s">
         <v>85</v>
       </c>
-      <c r="D29" s="348"/>
+      <c r="D29" s="335"/>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="C30" s="347" t="s">
+      <c r="C30" s="334" t="s">
         <v>87</v>
       </c>
-      <c r="D30" s="348"/>
+      <c r="D30" s="335"/>
     </row>
     <row r="31" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="C31" s="347" t="s">
+      <c r="C31" s="334" t="s">
         <v>89</v>
       </c>
-      <c r="D31" s="348"/>
+      <c r="D31" s="335"/>
     </row>
     <row r="32" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="C32" s="347" t="s">
+      <c r="C32" s="334" t="s">
         <v>91</v>
       </c>
-      <c r="D32" s="348"/>
+      <c r="D32" s="335"/>
     </row>
     <row r="33" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="C33" s="347" t="s">
+      <c r="C33" s="334" t="s">
         <v>93</v>
       </c>
-      <c r="D33" s="348"/>
+      <c r="D33" s="335"/>
     </row>
     <row r="34" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="C34" s="347" t="s">
+      <c r="C34" s="334" t="s">
         <v>95</v>
       </c>
-      <c r="D34" s="348"/>
+      <c r="D34" s="335"/>
     </row>
     <row r="35" spans="1:6" s="6" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="C35" s="340" t="s">
+      <c r="C35" s="332" t="s">
         <v>97</v>
       </c>
-      <c r="D35" s="341"/>
+      <c r="D35" s="333"/>
       <c r="E35" s="1"/>
       <c r="F35" s="25"/>
     </row>
@@ -7061,19 +7061,12 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="A8:A29"/>
     <mergeCell ref="C8:D8"/>
@@ -7090,12 +7083,19 @@
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7116,9 +7116,9 @@
   <dimension ref="A1:AF184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B33" sqref="B33"/>
-      <selection pane="bottomLeft" activeCell="D174" sqref="D174"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8012,9 +8012,11 @@
         <v>3</v>
       </c>
       <c r="E23" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="F23" s="54"/>
+        <v>71</v>
+      </c>
+      <c r="F23" s="325" t="s">
+        <v>520</v>
+      </c>
       <c r="G23" s="55" t="s">
         <v>110</v>
       </c>
@@ -8023,7 +8025,7 @@
       </c>
       <c r="AA23" s="319">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB23" s="319">
         <f t="shared" si="1"/>
@@ -8031,7 +8033,7 @@
       </c>
       <c r="AC23" s="319">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD23" s="319">
         <f t="shared" si="3"/>
@@ -14202,7 +14204,7 @@
       <c r="H174" s="238"/>
       <c r="AA174" s="82">
         <f>SUM(AA4:AA173)</f>
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AB174" s="82">
         <f>SUM(AB4:AB173)</f>
@@ -14210,7 +14212,7 @@
       </c>
       <c r="AC174" s="82">
         <f>SUM(AC4:AC173)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AD174" s="82">
         <f>SUM(AD4:AD173)</f>
@@ -14237,11 +14239,11 @@
       <c r="D178" s="73"/>
       <c r="E178" s="84">
         <f>AA174/F184</f>
-        <v>0.73750000000000004</v>
+        <v>0.73124999999999996</v>
       </c>
       <c r="F178">
         <f>AA174</f>
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
@@ -14267,11 +14269,11 @@
       <c r="D180" s="73"/>
       <c r="E180" s="84">
         <f>AC174/F184</f>
-        <v>0.10625</v>
+        <v>0.1125</v>
       </c>
       <c r="F180">
         <f>AC174</f>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.2">
@@ -19226,15 +19228,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Unknown Document Type" ma:contentTypeID="0x010104" ma:contentTypeVersion="0" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="05d83ceaa0bbd2e3bc716e6e66bd857a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b3d69fe45253d5ff147bb69036b756a7">
     <xsd:element name="properties">
@@ -19348,6 +19341,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -19355,14 +19357,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60846BC6-3376-492B-A137-BE9B817BCED1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD7F02ED-4036-4861-BDC4-1969BAC60D5E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19374,6 +19368,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60846BC6-3376-492B-A137-BE9B817BCED1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>